<commit_message>
Day 24 work in progress, before unified target map.
</commit_message>
<xml_diff>
--- a/src/december_17.xlsx
+++ b/src/december_17.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Documents\Advent_of_code\2024\obj\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Documents\Advent_of_code\2024\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{494412FF-A01F-45DB-8ECC-D12982D04BF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1268F9B6-D914-4A2A-8C12-C0E6E4381F38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="930" yWindow="3375" windowWidth="7500" windowHeight="12900" xr2:uid="{B07018A1-8CE6-4795-8EB9-ED1E4FBE7A1A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B07018A1-8CE6-4795-8EB9-ED1E4FBE7A1A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,9 +39,6 @@
     <t>IP</t>
   </si>
   <si>
-    <t>Insreuction</t>
-  </si>
-  <si>
     <t>bst (4) B := A mod 8</t>
   </si>
   <si>
@@ -67,6 +64,9 @@
   </si>
   <si>
     <t>bxc (X) B := C xor B</t>
+  </si>
+  <si>
+    <t>Instruction</t>
   </si>
 </sst>
 </file>
@@ -420,8 +420,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB51E828-6A6B-4644-8F7F-5FC5A4A646B6}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -436,10 +436,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -450,7 +450,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -469,7 +469,7 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -488,7 +488,7 @@
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -507,7 +507,7 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -526,7 +526,7 @@
         <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -545,7 +545,7 @@
         <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -564,7 +564,7 @@
         <v>0</v>
       </c>
       <c r="C14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -583,7 +583,7 @@
         <v>3</v>
       </c>
       <c r="C16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>